<commit_message>
fix shape sheet info about calendars
</commit_message>
<xml_diff>
--- a/Data/book.xlsx
+++ b/Data/book.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\github\ShapeSheetWatch\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Documents\GitHub\ShapeSheetWatch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3427" uniqueCount="1199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3430" uniqueCount="1200">
   <si>
     <t>Geometry</t>
   </si>
@@ -3620,6 +3620,9 @@
   </si>
   <si>
     <t>0-3</t>
+  </si>
+  <si>
+    <t>0=Western;1=Arabic Hijri;2=Hebrew Lunar;3=Taiwan Calendar;4=Japanese Emperor Reign;5=Thai Buddhist;6=Korean Danki;7=Saka Era;8=English transliterated;9=French transliterated</t>
   </si>
 </sst>
 </file>
@@ -3793,9 +3796,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="2" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4078,9 +4081,11 @@
   </sheetPr>
   <dimension ref="A1:K435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D396" workbookViewId="0">
+      <selection activeCell="J417" sqref="J417"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -12019,10 +12024,12 @@
       <c r="I229" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="J229" s="7"/>
+      <c r="J229" s="2" t="s">
+        <v>1199</v>
+      </c>
       <c r="K229" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>{11,L"Miscellaneous",L"",L"Calendar",visSectionObject,visRowMisc,visObjCalendar,L"Calendar",L""},</v>
+        <v>{11,L"Miscellaneous",L"",L"Calendar",visSectionObject,visRowMisc,visObjCalendar,L"Calendar",L"0=Western;1=Arabic Hijri;2=Hebrew Lunar;3=Taiwan Calendar;4=Japanese Emperor Reign;5=Thai Buddhist;6=Korean Danki;7=Saka Era;8=English transliterated;9=French transliterated"},</v>
       </c>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.2">
@@ -16765,10 +16772,12 @@
       <c r="I367" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="J367" s="8"/>
+      <c r="J367" s="8" t="s">
+        <v>1199</v>
+      </c>
       <c r="K367" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>{11,L"Shape Data",L"{r}",L"Calendar",visSectionProp,visRowProp ,visCustPropsCalendar,L"Prop.{r}.Calendar",L""},</v>
+        <v>{11,L"Shape Data",L"{r}",L"Calendar",visSectionProp,visRowProp ,visCustPropsCalendar,L"Prop.{r}.Calendar",L"0=Western;1=Arabic Hijri;2=Hebrew Lunar;3=Taiwan Calendar;4=Japanese Emperor Reign;5=Thai Buddhist;6=Korean Danki;7=Saka Era;8=English transliterated;9=French transliterated"},</v>
       </c>
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.2">
@@ -18489,10 +18498,12 @@
       <c r="I417" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="J417" s="12"/>
+      <c r="J417" s="12" t="s">
+        <v>1199</v>
+      </c>
       <c r="K417" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>{0,L"Text Fields",L"{i}",L"Calendar",visSectionTextField,visRowField ,visFieldCalendar,L"Fields.Calendar[{i}]",L""},</v>
+        <v>{0,L"Text Fields",L"{i}",L"Calendar",visSectionTextField,visRowField ,visFieldCalendar,L"Fields.Calendar[{i}]",L"0=Western;1=Arabic Hijri;2=Hebrew Lunar;3=Taiwan Calendar;4=Japanese Emperor Reign;5=Thai Buddhist;6=Korean Danki;7=Saka Era;8=English transliterated;9=French transliterated"},</v>
       </c>
     </row>
     <row r="418" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -19122,7 +19133,7 @@
       <selection activeCell="A236" sqref="A236"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
fix invalid shapesheet info
</commit_message>
<xml_diff>
--- a/Data/book.xlsx
+++ b/Data/book.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Documents\GitHub\ShapeSheetWatch\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\github\ShapeSheetWatch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3430" uniqueCount="1200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3430" uniqueCount="1201">
   <si>
     <t>Geometry</t>
   </si>
@@ -3623,6 +3623,9 @@
   </si>
   <si>
     <t>0=Western;1=Arabic Hijri;2=Hebrew Lunar;3=Taiwan Calendar;4=Japanese Emperor Reign;5=Thai Buddhist;6=Korean Danki;7=Saka Era;8=English transliterated;9=French transliterated</t>
+  </si>
+  <si>
+    <t>AvenueSizeX</t>
   </si>
 </sst>
 </file>
@@ -3796,9 +3799,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
-    <cellStyle name="Gut" xfId="1" builtinId="26"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4081,11 +4084,11 @@
   </sheetPr>
   <dimension ref="A1:K435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D396" workbookViewId="0">
-      <selection activeCell="J417" sqref="J417"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="F250" sqref="F250"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -12690,14 +12693,14 @@
         <v>20</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>44</v>
+        <v>1200</v>
       </c>
       <c r="D249" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E249" s="1"/>
       <c r="F249" s="1" t="s">
-        <v>44</v>
+        <v>1200</v>
       </c>
       <c r="G249" s="1" t="s">
         <v>10</v>
@@ -12711,7 +12714,7 @@
       <c r="J249" s="7"/>
       <c r="K249" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>{0,L"Page Layout",L"",L"AvenueSizeY",visSectionObject,visRowPageLayout,visPLOAvenueSizeX,L"AvenueSizeY",L""},</v>
+        <v>{0,L"Page Layout",L"",L"AvenueSizeX",visSectionObject,visRowPageLayout,visPLOAvenueSizeX,L"AvenueSizeX",L""},</v>
       </c>
     </row>
     <row r="250" spans="1:11" x14ac:dyDescent="0.2">
@@ -19133,7 +19136,7 @@
       <selection activeCell="A236" sqref="A236"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>

</xml_diff>